<commit_message>
Add new file data
</commit_message>
<xml_diff>
--- a/Data/draw_result_mega.xlsx
+++ b/Data/draw_result_mega.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1181"/>
+  <dimension ref="A1:H1187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45319,6 +45319,234 @@
         </is>
       </c>
     </row>
+    <row r="1182">
+      <c r="A1182" t="n">
+        <v>1181</v>
+      </c>
+      <c r="B1182" s="2" t="n">
+        <v>45387</v>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E1182" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F1182" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="G1182" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="H1182" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="n">
+        <v>1182</v>
+      </c>
+      <c r="B1183" s="2" t="n">
+        <v>45389</v>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E1183" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F1183" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="G1183" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H1183" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="n">
+        <v>1183</v>
+      </c>
+      <c r="B1184" s="2" t="n">
+        <v>45392</v>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F1184" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="G1184" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="H1184" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="n">
+        <v>1184</v>
+      </c>
+      <c r="B1185" s="2" t="n">
+        <v>45394</v>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F1185" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="G1185" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="H1185" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="n">
+        <v>1185</v>
+      </c>
+      <c r="B1186" s="2" t="n">
+        <v>45396</v>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F1186" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="G1186" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="H1186" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="n">
+        <v>1186</v>
+      </c>
+      <c r="B1187" s="2" t="n">
+        <v>45399</v>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="F1187" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="G1187" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="H1187" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>